<commit_message>
Ajustes na sequencia de inserir cotacao na planilha
</commit_message>
<xml_diff>
--- a/processando/planilhaInsereCotacao.xlsx
+++ b/processando/planilhaInsereCotacao.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F634C623-F24F-478D-A87A-A6A70AE7C403}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121A4B94-265D-43C2-887A-D9EBDDC75BD9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Cotação Euro</t>
   </si>
   <si>
     <t>Cotação Dólar</t>
+  </si>
+  <si>
+    <t>R$ 6.1482</t>
+  </si>
+  <si>
+    <t>R$ 5.188</t>
   </si>
 </sst>
 </file>
@@ -380,11 +386,11 @@
       </c>
     </row>
     <row r="2" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M2" s="2">
-        <v>6.1482000000000001</v>
+      <c r="M2" s="2" t="s">
+        <v>2</v>
       </c>
-      <c r="N2" s="2">
-        <v>5.1879999999999997</v>
+      <c r="N2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>